<commit_message>
Updated data cleaning to harmonize nutrients
</commit_message>
<xml_diff>
--- a/nutrients_highlightedwithconstraints.xlsx
+++ b/nutrients_highlightedwithconstraints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\G2 Classes\MIT15.053\project\optimization-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e29ea391e1dfcaac/MIT/15.053 Optimization/optimization-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B584119C-E9A3-400A-A3B9-71AC125FCBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{B584119C-E9A3-400A-A3B9-71AC125FCBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E284D5D1-2F34-6341-80A6-58A2007C83A2}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="13590" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="41820" yWindow="13600" windowWidth="34980" windowHeight="23620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nutrients" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1012,21 +1012,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="21.26171875" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="15.15625" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1039,212 +1040,212 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>